<commit_message>
Updated MainMenu for OPG7 with more functions
</commit_message>
<xml_diff>
--- a/SDE/OPG7/VM.xlsx
+++ b/SDE/OPG7/VM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -39,12 +39,6 @@
     <t>CPUCount</t>
   </si>
   <si>
-    <t>VMPath</t>
-  </si>
-  <si>
-    <t>ISOPath</t>
-  </si>
-  <si>
     <t>D:\Test-v</t>
   </si>
   <si>
@@ -79,6 +73,21 @@
   </si>
   <si>
     <t>OtherVHDSizeGB</t>
+  </si>
+  <si>
+    <t>vSwitch</t>
+  </si>
+  <si>
+    <t>External Switch</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>D:\Hyper-V</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -493,14 +502,14 @@
     <col min="5" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.109375" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -515,16 +524,19 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -544,15 +556,18 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -567,18 +582,21 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -593,15 +611,18 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -616,15 +637,18 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -639,15 +663,18 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -662,18 +689,21 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -688,15 +718,18 @@
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -711,15 +744,18 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -731,10 +767,13 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>